<commit_message>
Updates to support PR comments
* Cleanup import handling
* Switch fo ISO date formats
</commit_message>
<xml_diff>
--- a/examples/schedule_prep_spreadsheet.xlsx
+++ b/examples/schedule_prep_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpadams/proj/pds/pdsen/workspace/lasso-issues/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FD416843-FF74-784D-AE14-05E39307B096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AD673B-01B4-3940-A39D-E28B3B95C480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="940" windowWidth="33240" windowHeight="15540" activeTab="1" xr2:uid="{77BE7B00-5D39-0F40-9AE5-E33691EB16DC}"/>
+    <workbookView xWindow="1200" yWindow="940" windowWidth="33240" windowHeight="15540" activeTab="2" xr2:uid="{77BE7B00-5D39-0F40-9AE5-E33691EB16DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Date" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Baseline!$A$1:$H$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -287,6 +287,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -323,14 +326,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +669,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +678,7 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="4">
         <v>46177</v>
       </c>
     </row>
@@ -691,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A282D7-36CC-A540-8420-FCD049761715}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,15 +751,15 @@
       <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <f t="shared" ref="C2:C3" si="0">D2-E2</f>
         <v>45905</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <f>'Release Date'!$B$1-F2</f>
         <v>45946</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>41</v>
       </c>
       <c r="F2">
@@ -786,15 +787,15 @@
       <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <f t="shared" si="0"/>
         <v>45926</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <f>'Release Date'!$B$1-F3</f>
         <v>46093</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>167</v>
       </c>
       <c r="F3">
@@ -816,15 +817,15 @@
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <f t="shared" ref="C4" si="1">D4-E4</f>
         <v>45926</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <f>'Release Date'!$B$1-F4</f>
         <v>46093</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>167</v>
       </c>
       <c r="F4">
@@ -852,15 +853,15 @@
       <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <f t="shared" ref="C5:C6" si="2">D5-E5</f>
         <v>45926</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <f>'Release Date'!$B$1-F5</f>
         <v>46093</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>167</v>
       </c>
       <c r="F5">
@@ -888,15 +889,15 @@
       <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <f t="shared" si="2"/>
         <v>45926</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <f>'Release Date'!$B$1-F6</f>
         <v>46093</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>167</v>
       </c>
       <c r="F6">
@@ -925,15 +926,15 @@
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <f t="shared" ref="C7:C19" si="3">D7-E7</f>
         <v>45926</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <f>'Release Date'!$B$1-F7</f>
         <v>46093</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>167</v>
       </c>
       <c r="F7">
@@ -962,11 +963,11 @@
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <f t="shared" si="3"/>
         <v>45926</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <f>'Release Date'!$B$1-F8</f>
         <v>46114</v>
       </c>
@@ -999,11 +1000,11 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <f t="shared" si="3"/>
         <v>46093</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <f>'Release Date'!$B$1-F9</f>
         <v>46093</v>
       </c>
@@ -1036,11 +1037,11 @@
       <c r="B10" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <f t="shared" ref="C10:C11" si="4">D10-E10</f>
         <v>46094</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <f>'Release Date'!$B$1-F10</f>
         <v>46114</v>
       </c>
@@ -1076,11 +1077,11 @@
       <c r="B11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <f t="shared" si="4"/>
         <v>46094</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <f>'Release Date'!$B$1-F11</f>
         <v>46114</v>
       </c>
@@ -1107,11 +1108,11 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <f t="shared" si="3"/>
         <v>46094</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <f>'Release Date'!$B$1-F12</f>
         <v>46114</v>
       </c>
@@ -1147,11 +1148,11 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <f t="shared" si="3"/>
         <v>46094</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <f>'Release Date'!$B$1-F13</f>
         <v>46114</v>
       </c>
@@ -1187,11 +1188,11 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <f t="shared" si="3"/>
         <v>46115</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <f>'Release Date'!$B$1-F14</f>
         <v>46156</v>
       </c>
@@ -1227,11 +1228,11 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <f t="shared" si="3"/>
         <v>46115</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <f>'Release Date'!$B$1-F15</f>
         <v>46156</v>
       </c>
@@ -1267,11 +1268,11 @@
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f t="shared" si="3"/>
         <v>46115</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <f>'Release Date'!$B$1-F16</f>
         <v>46156</v>
       </c>
@@ -1307,11 +1308,11 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <f t="shared" si="3"/>
         <v>46115</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <f>'Release Date'!$B$1-F17</f>
         <v>46136</v>
       </c>
@@ -1344,11 +1345,11 @@
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="3"/>
         <v>46136</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <f>'Release Date'!$B$1-F18</f>
         <v>46177</v>
       </c>
@@ -1384,11 +1385,11 @@
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <f t="shared" si="3"/>
         <v>46157</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <f>'Release Date'!$B$1-F19</f>
         <v>46177</v>
       </c>
@@ -1418,7 +1419,36 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D20" s="1"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1429,53 +1459,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1773B976-BCDA-D945-919B-7C561A0B150A}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="23.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="4">
@@ -1484,21 +1513,21 @@
       <c r="D2" s="4">
         <v>45778</v>
       </c>
-      <c r="E2" s="5">
-        <f>_xlfn.DAYS(D2,C2)</f>
+      <c r="E2" s="2">
+        <f t="shared" ref="E2:E17" si="0">_xlfn.DAYS(D2,C2)</f>
         <v>41</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D2)</f>
         <v>399</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4">
@@ -1507,21 +1536,21 @@
       <c r="D3" s="4">
         <v>45946</v>
       </c>
-      <c r="E3" s="5">
-        <f>_xlfn.DAYS(D3,C3)</f>
+      <c r="E3" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D3)</f>
         <v>231</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="4">
@@ -1530,21 +1559,21 @@
       <c r="D4" s="4">
         <v>45946</v>
       </c>
-      <c r="E4" s="5">
-        <f>_xlfn.DAYS(D4,C4)</f>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
         <v>189</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D4)</f>
         <v>231</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4">
@@ -1553,23 +1582,23 @@
       <c r="D5" s="4">
         <v>45926</v>
       </c>
-      <c r="E5" s="5">
-        <f>_xlfn.DAYS(D5,C5)</f>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D5)</f>
         <v>251</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="4">
@@ -1578,26 +1607,26 @@
       <c r="D6" s="4">
         <v>45946</v>
       </c>
-      <c r="E6" s="5">
-        <f>_xlfn.DAYS(D6,C6)</f>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D6)</f>
         <v>231</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="4">
@@ -1606,24 +1635,24 @@
       <c r="D7" s="4">
         <v>45946</v>
       </c>
-      <c r="E7" s="5">
-        <f>_xlfn.DAYS(D7,C7)</f>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D7)</f>
         <v>231</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4">
@@ -1632,26 +1661,26 @@
       <c r="D8" s="4">
         <v>45988</v>
       </c>
-      <c r="E8" s="5">
-        <f>_xlfn.DAYS(D8,C8)</f>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D8)</f>
         <v>189</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4">
@@ -1660,26 +1689,26 @@
       <c r="D9" s="4">
         <v>45988</v>
       </c>
-      <c r="E9" s="5">
-        <f>_xlfn.DAYS(D9,C9)</f>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D9)</f>
         <v>189</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="4">
@@ -1688,26 +1717,26 @@
       <c r="D10" s="4">
         <v>45988</v>
       </c>
-      <c r="E10" s="5">
-        <f>_xlfn.DAYS(D10,C10)</f>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D10)</f>
         <v>189</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4">
@@ -1716,23 +1745,23 @@
       <c r="D11" s="4">
         <v>45967</v>
       </c>
-      <c r="E11" s="5">
-        <f>_xlfn.DAYS(D11,C11)</f>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D11)</f>
         <v>210</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4">
@@ -1741,26 +1770,26 @@
       <c r="D12" s="4">
         <v>46009</v>
       </c>
-      <c r="E12" s="5">
-        <f>_xlfn.DAYS(D12,C12)</f>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D12)</f>
         <v>168</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4">
@@ -1769,52 +1798,52 @@
       <c r="D13" s="4">
         <v>46009</v>
       </c>
-      <c r="E13" s="5">
-        <f>_xlfn.DAYS(D13,C13)</f>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <f>_xlfn.DAYS('Release Date'!$B$1,D13)</f>
         <v>168</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E14" s="5">
-        <f>_xlfn.DAYS(D14,C14)</f>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="5">
-        <f>_xlfn.DAYS(D15,C15)</f>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E16" s="5">
-        <f>_xlfn.DAYS(D16,C16)</f>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E17" s="5">
-        <f>_xlfn.DAYS(D17,C17)</f>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H13" xr:uid="{1773B976-BCDA-D945-919B-7C561A0B150A}">

</xml_diff>

<commit_message>
Update spreadsheet template to include
</commit_message>
<xml_diff>
--- a/examples/schedule_prep_spreadsheet.xlsx
+++ b/examples/schedule_prep_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpadams/proj/pds/pdsen/workspace/lasso-issues/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AD673B-01B4-3940-A39D-E28B3B95C480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B8CAF-0916-CC42-959C-D375AB02026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="940" windowWidth="33240" windowHeight="15540" activeTab="2" xr2:uid="{77BE7B00-5D39-0F40-9AE5-E33691EB16DC}"/>
+    <workbookView xWindow="1200" yWindow="940" windowWidth="33240" windowHeight="15540" activeTab="1" xr2:uid="{77BE7B00-5D39-0F40-9AE5-E33691EB16DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Date" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
   <si>
     <t xml:space="preserve">Task </t>
   </si>
@@ -199,24 +199,6 @@
     <t>LOE support for high priority improvements to Data Upload Manager</t>
   </si>
   <si>
-    <t>Validate Support: High Priority Enhancements / Bug Fixes / Tasks</t>
-  </si>
-  <si>
-    <t>Registry API Support: High Priority Enhancements / Bug Fixes / Tasks</t>
-  </si>
-  <si>
-    <t>DUM Support:  High Priority Enhancements / Bug Fixes / Tasks</t>
-  </si>
-  <si>
-    <t>Registry Support: High Priority Enhancements / Bug Fixes / Tasks</t>
-  </si>
-  <si>
-    <t>SCR Freeze</t>
-  </si>
-  <si>
-    <t>dLDD Integration &amp; Test</t>
-  </si>
-  <si>
     <t>Deployment of Test Environment;Deployment of Production Environment - https://docs.google.com/spreadsheets/d/1f1zK9hdR3RWQP9PiR80EMFQ3xDqca1tK2a7oqSCKuHE/edit?usp=sharing;Webpage Updated - documents , discipline LDDs, TBD mission LDDs;Release announcement to public</t>
   </si>
   <si>
@@ -253,9 +235,6 @@
     <t>Security Scan</t>
   </si>
   <si>
-    <t>Triage Security Code Scans</t>
-  </si>
-  <si>
     <t>NASA-PDS/planetary-data-cloud</t>
   </si>
   <si>
@@ -268,9 +247,6 @@
     <t>Triage Security Code Scans from SonarCloud</t>
   </si>
   <si>
-    <t>Registry Legacy Support: High Priority Enhancements / Bug Fixes / Tasks</t>
-  </si>
-  <si>
     <t>NASA-PDS/registry-legacy-solr</t>
   </si>
   <si>
@@ -280,7 +256,58 @@
     <t>Cloud Operations</t>
   </si>
   <si>
-    <t>Bi-annual Cloud Resource Housekeeping</t>
+    <t>$BUILD Release Planning</t>
+  </si>
+  <si>
+    <t>$BUILD Registry Legacy Support: High Priority Enhancements / Bug Fixes / Tasks</t>
+  </si>
+  <si>
+    <t>$BUILD Validate Support: High Priority Enhancements / Bug Fixes / Tasks</t>
+  </si>
+  <si>
+    <t>$BUILD Registry API Support: High Priority Enhancements / Bug Fixes / Tasks</t>
+  </si>
+  <si>
+    <t>$BUILD DUM Support:  High Priority Enhancements / Bug Fixes / Tasks</t>
+  </si>
+  <si>
+    <t>$BUILD Registry Support: High Priority Enhancements / Bug Fixes / Tasks</t>
+  </si>
+  <si>
+    <t>$BUILD Information Model SCR Implementation and LDDTool Updates</t>
+  </si>
+  <si>
+    <t>$BUILD SCR Freeze</t>
+  </si>
+  <si>
+    <t>$BUILD Triage Security Code Scans</t>
+  </si>
+  <si>
+    <t>$BUILD Bi-annual Cloud Resource Housekeeping</t>
+  </si>
+  <si>
+    <t>$BUILD Information Model Delivery to I&amp;T</t>
+  </si>
+  <si>
+    <t>$BUILD dLDD Integration &amp; Test</t>
+  </si>
+  <si>
+    <t>$BUILD Standards Documents Updates</t>
+  </si>
+  <si>
+    <t>$BUILD Standards Document Review</t>
+  </si>
+  <si>
+    <t>$BUILD Information Model I&amp;T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$BUILD System Integration &amp; Test </t>
+  </si>
+  <si>
+    <t>$BUILD Delivery &amp; Deployment Review (DDR)</t>
+  </si>
+  <si>
+    <t>$BUILD Deployment and Release</t>
   </si>
 </sst>
 </file>
@@ -288,7 +315,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -331,7 +358,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A282D7-36CC-A540-8420-FCD049761715}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,7 +738,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -735,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
         <v>43</v>
@@ -746,10 +773,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4">
         <f t="shared" ref="C2:C3" si="0">D2-E2</f>
@@ -769,7 +796,7 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J2" s="2" t="b">
         <f>IF(C2="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C2+20)),21)=0))</f>
@@ -782,10 +809,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" si="0"/>
@@ -802,17 +829,17 @@
         <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -848,7 +875,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -871,7 +898,7 @@
         <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J5" s="2" t="b">
         <f>IF(C5="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C5+20)),21)=0))</f>
@@ -884,7 +911,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -907,7 +934,7 @@
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J6" s="2" t="b">
         <f>IF(C6="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C6+20)),21)=0))</f>
@@ -921,7 +948,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -944,7 +971,7 @@
         <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="b">
         <f>IF(C7="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C7+20)),21)=0))</f>
@@ -958,7 +985,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -981,7 +1008,7 @@
         <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J8" s="2" t="b">
         <f>IF(C8="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C8+20)),21)=0))</f>
@@ -995,7 +1022,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1018,7 +1045,7 @@
         <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J9" s="2" t="b">
         <f>IF(C9="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C9+20)),21)=0))</f>
@@ -1032,10 +1059,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" ref="C10:C11" si="4">D10-E10</f>
@@ -1052,13 +1079,13 @@
         <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J10" s="2" t="b">
         <f>IF(C10="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C10+20)),21)=0))</f>
@@ -1072,10 +1099,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="4"/>
@@ -1092,10 +1119,10 @@
         <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1103,7 +1130,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1129,7 +1156,7 @@
         <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J12" s="2" t="b">
         <f>IF(C12="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C12+20)),21)=0))</f>
@@ -1143,7 +1170,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1169,7 +1196,7 @@
         <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J13" s="2" t="b">
         <f>IF(C13="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C13+20)),21)=0))</f>
@@ -1183,7 +1210,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1209,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J14" s="2" t="b">
         <f>IF(C14="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C14+20)),21)=0))</f>
@@ -1223,7 +1250,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -1249,7 +1276,7 @@
         <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J15" s="2" t="b">
         <f>IF(C15="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C15+20)),21)=0))</f>
@@ -1263,7 +1290,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1289,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J16" s="2" t="b">
         <f>IF(C16="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C16+20)),21)=0))</f>
@@ -1303,7 +1330,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1326,7 +1353,7 @@
         <v>23</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J17" s="2" t="b">
         <f>IF(C17="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C17+20)),21)=0))</f>
@@ -1340,7 +1367,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -1366,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J18" s="2" t="b">
         <f>IF(C18="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C18+20)),21)=0))</f>
@@ -1380,7 +1407,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1403,10 +1430,10 @@
         <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J19" s="2" t="b">
         <f>IF(C19="","",(MOD(_xlfn.DAYS('Release Date'!$B$1,(C19+20)),21)=0))</f>
@@ -1459,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1773B976-BCDA-D945-919B-7C561A0B150A}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1502,10 +1529,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4">
         <v>45737</v>
@@ -1525,7 +1552,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>

</xml_diff>